<commit_message>
committing few changes in Obligation suite files- Naveen Task
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Obligation Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Obligation Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1489,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,8 +2323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2556,7 +2556,7 @@
         <v>174</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>282</v>
+        <v>175</v>
       </c>
       <c r="R2" s="19" t="s">
         <v>286</v>

</xml_diff>